<commit_message>
add folder in ignore file
</commit_message>
<xml_diff>
--- a/files/excels/schools/tmp/Список - 2021.xlsx
+++ b/files/excels/schools/tmp/Список - 2021.xlsx
@@ -11,7 +11,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="34">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="28">
   <si>
     <t>ФИО</t>
   </si>
@@ -64,55 +64,37 @@
     <t>Ахмедов Ахмед Ахмедович</t>
   </si>
   <si>
-    <t>09-12-2000</t>
+    <t>01-08-1988</t>
   </si>
   <si>
     <t>Грозненский район</t>
   </si>
   <si>
-    <t>МБОУ Тестовая школа</t>
+    <t>МБОУ средняя общеобразовательная школа с.Виноградное</t>
   </si>
   <si>
     <t xml:space="preserve">Учитель математики </t>
   </si>
   <si>
-    <t>педагог</t>
+    <t>Экономист</t>
   </si>
   <si>
     <t>ЧИПКРО</t>
   </si>
   <si>
-    <t>2020</t>
+    <t>2019</t>
   </si>
   <si>
     <t>первая</t>
   </si>
   <si>
-    <t>akhmedov@akhmedov.ru</t>
-  </si>
-  <si>
-    <t>+79991112221</t>
+    <t>vinogradovskayasos1h@mail.ru</t>
+  </si>
+  <si>
+    <t>89991118888</t>
   </si>
   <si>
     <t>Мужской</t>
-  </si>
-  <si>
-    <t>Саидов Саид Саидович</t>
-  </si>
-  <si>
-    <t>30-10-2020</t>
-  </si>
-  <si>
-    <t>Учитель русского языка и литературы</t>
-  </si>
-  <si>
-    <t/>
-  </si>
-  <si>
-    <t>webrush@mail.ru</t>
-  </si>
-  <si>
-    <t>+79991440788</t>
   </si>
 </sst>
 </file>
@@ -489,7 +471,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:P3"/>
+  <dimension ref="A1:P2"/>
   <sheetFormatPr defaultRowHeight="15" outlineLevelRow="0" outlineLevelCol="0" x14ac:dyDescent="55"/>
   <cols>
     <col min="1" max="1" width="40" customWidth="1"/>
@@ -562,7 +544,7 @@
         <v>11111111111</v>
       </c>
       <c r="D2">
-        <v>21</v>
+        <v>33</v>
       </c>
       <c r="E2" t="s">
         <v>18</v>
@@ -577,10 +559,10 @@
         <v>21</v>
       </c>
       <c r="I2">
-        <v>2</v>
+        <v>10</v>
       </c>
       <c r="J2">
-        <v>2</v>
+        <v>10</v>
       </c>
       <c r="K2" t="s">
         <v>22</v>
@@ -598,56 +580,6 @@
         <v>26</v>
       </c>
       <c r="P2" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="3" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
-        <v>28</v>
-      </c>
-      <c r="B3" t="s">
-        <v>29</v>
-      </c>
-      <c r="C3">
-        <v>11111111111</v>
-      </c>
-      <c r="D3">
-        <v>1</v>
-      </c>
-      <c r="E3" t="s">
-        <v>18</v>
-      </c>
-      <c r="F3" t="s">
-        <v>19</v>
-      </c>
-      <c r="G3" t="s">
-        <v>30</v>
-      </c>
-      <c r="H3" t="s">
-        <v>31</v>
-      </c>
-      <c r="I3">
-        <v>0</v>
-      </c>
-      <c r="J3">
-        <v>0</v>
-      </c>
-      <c r="K3" t="s">
-        <v>31</v>
-      </c>
-      <c r="L3" t="s">
-        <v>31</v>
-      </c>
-      <c r="M3" t="s">
-        <v>24</v>
-      </c>
-      <c r="N3" t="s">
-        <v>32</v>
-      </c>
-      <c r="O3" t="s">
-        <v>33</v>
-      </c>
-      <c r="P3" t="s">
         <v>27</v>
       </c>
     </row>

</xml_diff>